<commit_message>
fix: Add `Icon` column for 1F.
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078C35A4-BACC-40BD-9C15-A18B86F73C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" r:id="rId1"/>
-    <sheet name="1" sheetId="2" r:id="rId2"/>
+    <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="1" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -26,42 +21,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="82">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Slug</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>Sitrus</t>
-  </si>
-  <si>
-    <t>store</t>
-  </si>
-  <si>
-    <t>sitrus</t>
-  </si>
-  <si>
-    <t>The Flows Gourmet</t>
-  </si>
-  <si>
-    <t>restaurant</t>
-  </si>
-  <si>
-    <t>the-flows-gourmet</t>
-  </si>
-  <si>
-    <t>蜀都风味</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitrus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sitrus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Flows Gourmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the-flows-gourmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蜀都风味</t>
   </si>
   <si>
     <r>
@@ -81,7 +76,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>闽桂中国超市</t>
+      <t xml:space="preserve">闽桂中国超市</t>
     </r>
   </si>
   <si>
@@ -102,7 +97,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>薯嘟嘟超市</t>
+      <t xml:space="preserve">薯嘟嘟超市</t>
     </r>
   </si>
   <si>
@@ -122,17 +117,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>车店</t>
-    </r>
-  </si>
-  <si>
-    <t>misc</t>
-  </si>
-  <si>
-    <t>DirectionsCarFilledRoundedIcon</t>
-  </si>
-  <si>
-    <t>The Grind</t>
+      <t xml:space="preserve">车店</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">misc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DirectionsCarFilledRoundedIcon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Grind</t>
   </si>
   <si>
     <r>
@@ -152,7 +147,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>食坊</t>
+      <t xml:space="preserve">食坊</t>
     </r>
   </si>
   <si>
@@ -173,7 +168,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>礼品店</t>
+      <t xml:space="preserve">礼品店</t>
     </r>
   </si>
   <si>
@@ -194,17 +189,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>宠物诊所</t>
-    </r>
-  </si>
-  <si>
-    <t>KIMS SALON</t>
-  </si>
-  <si>
-    <t>Starbucks</t>
-  </si>
-  <si>
-    <t>coffee</t>
+      <t xml:space="preserve">宠物诊所</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">KIMS SALON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starbucks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coffee</t>
   </si>
   <si>
     <r>
@@ -224,7 +219,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>华莱士</t>
+      <t xml:space="preserve">华莱士</t>
     </r>
   </si>
   <si>
@@ -245,14 +240,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>蜜雪冰城</t>
-    </r>
-  </si>
-  <si>
-    <t>drink</t>
-  </si>
-  <si>
-    <t>KK</t>
+      <t xml:space="preserve">蜜雪冰城</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">drink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KK</t>
   </si>
   <si>
     <r>
@@ -272,7 +267,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>冰雪时光</t>
+      <t xml:space="preserve">冰雪时光</t>
     </r>
   </si>
   <si>
@@ -296,7 +291,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>鸿运租车</t>
+      <t xml:space="preserve">鸿运租车</t>
     </r>
   </si>
   <si>
@@ -317,20 +312,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>新式快炒</t>
-    </r>
-  </si>
-  <si>
-    <t>沙县小吃</t>
-  </si>
-  <si>
-    <t>PaoPaoPot</t>
-  </si>
-  <si>
-    <t>Secret Recipe</t>
-  </si>
-  <si>
-    <t>snack</t>
+      <t xml:space="preserve">新式快炒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">沙县小吃</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PaoPaoPot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secret Recipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snack</t>
   </si>
   <si>
     <r>
@@ -350,7 +345,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>面对面</t>
+      <t xml:space="preserve">面对面</t>
     </r>
   </si>
   <si>
@@ -371,14 +366,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>麻辣诱惑</t>
-    </r>
-  </si>
-  <si>
-    <t>The Daily Kueh</t>
-  </si>
-  <si>
-    <t>聚椒
+      <t xml:space="preserve">麻辣诱惑</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The Daily Kueh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">聚椒
 烤肉火锅店</t>
   </si>
   <si>
@@ -398,20 +393,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>甜点</t>
-    </r>
-  </si>
-  <si>
-    <t>洗衣房</t>
-  </si>
-  <si>
-    <t>申通快递</t>
-  </si>
-  <si>
-    <t>Black 8 Internatinoal Club</t>
-  </si>
-  <si>
-    <t>entertainment</t>
+      <t xml:space="preserve">甜点</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">洗衣房</t>
+  </si>
+  <si>
+    <t xml:space="preserve">申通快递</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black 8 Internatinoal Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entertainment</t>
   </si>
   <si>
     <r>
@@ -431,7 +426,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>ZEKUN TCM HEALTHCARE</t>
+      <t xml:space="preserve">ZEKUN TCM HEALTHCARE</t>
     </r>
   </si>
   <si>
@@ -452,17 +447,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Xinjiang Restaurant</t>
-    </r>
-  </si>
-  <si>
-    <t>Event Space</t>
-  </si>
-  <si>
-    <t>百家牛肉面</t>
-  </si>
-  <si>
-    <t>Baskin Robbins BR</t>
+      <t xml:space="preserve">Xinjiang Restaurant</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Event Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">百家牛肉面</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baskin Robbins BR</t>
   </si>
   <si>
     <r>
@@ -482,7 +477,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>冰室</t>
+      <t xml:space="preserve">冰室</t>
     </r>
   </si>
   <si>
@@ -503,29 +498,29 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>ChaPanda</t>
-    </r>
-  </si>
-  <si>
-    <t>大圣烧烤</t>
-  </si>
-  <si>
-    <t>金龙牛肉煲仔饭</t>
-  </si>
-  <si>
-    <t>Vape Coffee</t>
-  </si>
-  <si>
-    <t>鸡公煲</t>
-  </si>
-  <si>
-    <t>笆篱是家大排档</t>
-  </si>
-  <si>
-    <t>茶作饮品店</t>
-  </si>
-  <si>
-    <t>佳粤</t>
+      <t xml:space="preserve">ChaPanda</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">大圣烧烤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金龙牛肉煲仔饭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vape Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鸡公煲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">笆篱是家大排档</t>
+  </si>
+  <si>
+    <t xml:space="preserve">茶作饮品店</t>
+  </si>
+  <si>
+    <t xml:space="preserve">佳粤</t>
   </si>
   <si>
     <r>
@@ -545,30 +540,30 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>一二爽便利咖</t>
-    </r>
-  </si>
-  <si>
-    <t>123express-mart</t>
-  </si>
-  <si>
-    <t>Nasi Kandar Mamak</t>
-  </si>
-  <si>
-    <t>mamak</t>
+      <t xml:space="preserve">一二爽便利咖</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">123express-mart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasi Kandar Mamak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mamak</t>
   </si>
   <si>
     <t xml:space="preserve">ChaZhuGong Milk tea
 </t>
   </si>
   <si>
-    <t>chazhugong-milk-tea</t>
-  </si>
-  <si>
-    <t>Cafe Lazatnyo</t>
-  </si>
-  <si>
-    <t>Gepreking Fried Kitchen</t>
+    <t xml:space="preserve">chazhugong-milk-tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cafe Lazatnyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gepreking Fried Kitchen</t>
   </si>
   <si>
     <r>
@@ -588,11 +583,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Stella Vet</t>
-    </r>
-  </si>
-  <si>
-    <t>CHATTO</t>
+      <t xml:space="preserve">Stella Vet</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CHATTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marqa Caff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marqacaff</t>
   </si>
   <si>
     <r>
@@ -612,7 +613,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Yoga</t>
+      <t xml:space="preserve">Yoga</t>
     </r>
   </si>
   <si>
@@ -633,11 +634,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Braised Chicken</t>
-    </r>
-  </si>
-  <si>
-    <t>Real Peak Music</t>
+      <t xml:space="preserve">Braised Chicken</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Peak Music</t>
   </si>
   <si>
     <r>
@@ -657,7 +658,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>People’s Bookstore</t>
+      <t xml:space="preserve">People’s Bookstore</t>
     </r>
   </si>
   <si>
@@ -678,7 +679,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Grilled Fish</t>
+      <t xml:space="preserve">Grilled Fish</t>
     </r>
   </si>
   <si>
@@ -699,7 +700,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Real Estate</t>
+      <t xml:space="preserve">Real Estate</t>
     </r>
   </si>
   <si>
@@ -719,11 +720,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>桌游店</t>
-    </r>
-  </si>
-  <si>
-    <t>SENZE CAFE</t>
+      <t xml:space="preserve">桌游店</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SENZE CAFE</t>
   </si>
   <si>
     <r>
@@ -743,7 +744,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Korean Speaking Class</t>
+      <t xml:space="preserve">Korean Speaking Class</t>
     </r>
   </si>
   <si>
@@ -764,7 +765,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>XILE DESSERT</t>
+      <t xml:space="preserve">XILE DESSERT</t>
     </r>
   </si>
   <si>
@@ -785,23 +786,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Billiard Hall</t>
-    </r>
-  </si>
-  <si>
-    <t>Marqa Caff</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>marqacaff</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+      <t xml:space="preserve">Billiard Hall</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -810,15 +806,24 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="LXGW WenKai Mono"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -830,112 +835,130 @@
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -988,26 +1011,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C78" activeCellId="0" sqref="C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16384" width="11.54296875" style="1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.75" customHeight="1">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1054,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="35.75" customHeight="1">
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1047,7 +1072,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="35.75" customHeight="1">
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1065,10 +1090,10 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="35.75" customHeight="1">
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D4" s="2"/>
@@ -1079,10 +1104,10 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="35.75" customHeight="1">
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D5" s="2"/>
@@ -1093,14 +1118,14 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="35.75" customHeight="1">
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D6" s="2"/>
@@ -1111,14 +1136,14 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="35.75" customHeight="1">
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D7" s="2"/>
@@ -1129,14 +1154,14 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="35.75" customHeight="1">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D8" s="2"/>
@@ -1147,17 +1172,17 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="35.75" customHeight="1">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2">
-        <v>404</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="2" t="n">
+        <v>404</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1169,10 +1194,10 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="35.75" customHeight="1">
+    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2">
+      <c r="C10" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D10" s="2"/>
@@ -1183,14 +1208,14 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="35.75" customHeight="1">
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D11" s="2"/>
@@ -1201,14 +1226,14 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="35.75" customHeight="1">
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D12" s="2"/>
@@ -1219,14 +1244,14 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="35.75" customHeight="1">
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D13" s="2"/>
@@ -1237,10 +1262,10 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="35.75" customHeight="1">
+    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2">
+      <c r="C14" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D14" s="2"/>
@@ -1251,14 +1276,14 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="35.75" customHeight="1">
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D15" s="2"/>
@@ -1269,14 +1294,14 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="35.75" customHeight="1">
-      <c r="A16" s="2">
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
         <v>711</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D16" s="2"/>
@@ -1287,14 +1312,14 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="35.75" customHeight="1">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D17" s="2"/>
@@ -1305,10 +1330,10 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="35.75" customHeight="1">
+    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2">
+      <c r="C18" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D18" s="2"/>
@@ -1319,10 +1344,10 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="35.75" customHeight="1">
+    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2">
+      <c r="C19" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D19" s="2"/>
@@ -1333,14 +1358,14 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="35.75" customHeight="1">
+    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D20" s="2"/>
@@ -1351,14 +1376,14 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="35.75" customHeight="1">
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D21" s="2"/>
@@ -1369,14 +1394,14 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="35.75" customHeight="1">
+    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D22" s="2"/>
@@ -1387,10 +1412,10 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="35.75" customHeight="1">
+    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2">
+      <c r="C23" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D23" s="2"/>
@@ -1401,14 +1426,14 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="35.75" customHeight="1">
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D24" s="2"/>
@@ -1419,10 +1444,10 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="35.75" customHeight="1">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2">
+      <c r="C25" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D25" s="2"/>
@@ -1433,14 +1458,14 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="35.75" customHeight="1">
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D26" s="2"/>
@@ -1451,10 +1476,10 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" ht="35.75" customHeight="1">
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2">
+      <c r="C27" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D27" s="2"/>
@@ -1465,14 +1490,14 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="35.75" customHeight="1">
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D28" s="2"/>
@@ -1483,14 +1508,14 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="35.75" customHeight="1">
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D29" s="2"/>
@@ -1501,14 +1526,14 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" ht="35.75" customHeight="1">
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D30" s="2"/>
@@ -1519,14 +1544,14 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="35.75" customHeight="1">
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D31" s="2"/>
@@ -1537,14 +1562,14 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" ht="35.75" customHeight="1">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D32" s="2"/>
@@ -1555,14 +1580,14 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="35.75" customHeight="1">
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D33" s="2"/>
@@ -1573,10 +1598,10 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" ht="35.75" customHeight="1">
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2">
+      <c r="C34" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D34" s="2"/>
@@ -1587,10 +1612,10 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" ht="35.75" customHeight="1">
+    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="2">
+      <c r="C35" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D35" s="2"/>
@@ -1601,14 +1626,14 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" ht="35.75" customHeight="1">
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D36" s="2"/>
@@ -1619,10 +1644,10 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="35.75" customHeight="1">
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="2">
+      <c r="C37" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D37" s="2"/>
@@ -1633,14 +1658,14 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="35.75" customHeight="1">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D38" s="2"/>
@@ -1651,14 +1676,14 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" ht="35.75" customHeight="1">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D39" s="2"/>
@@ -1669,10 +1694,10 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" ht="35.75" customHeight="1">
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="2">
+      <c r="C40" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D40" s="2"/>
@@ -1683,10 +1708,10 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="35.75" customHeight="1">
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="2">
+      <c r="C41" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D41" s="2"/>
@@ -1697,10 +1722,10 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" ht="35.75" customHeight="1">
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="2">
+      <c r="C42" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D42" s="2"/>
@@ -1711,10 +1736,10 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" ht="35.75" customHeight="1">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="2">
+      <c r="C43" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D43" s="2"/>
@@ -1725,10 +1750,10 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" ht="35.75" customHeight="1">
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
-      <c r="C44" s="2">
+      <c r="C44" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D44" s="2"/>
@@ -1739,10 +1764,10 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" ht="35.75" customHeight="1">
+    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2">
+      <c r="C45" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D45" s="2"/>
@@ -1753,10 +1778,10 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" ht="35.75" customHeight="1">
+    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="2">
+      <c r="C46" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D46" s="2"/>
@@ -1767,10 +1792,10 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" ht="35.75" customHeight="1">
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="2">
+      <c r="C47" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D47" s="2"/>
@@ -1781,10 +1806,10 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" ht="35.75" customHeight="1">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="2">
+      <c r="C48" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D48" s="2"/>
@@ -1795,10 +1820,10 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" ht="35.75" customHeight="1">
+    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="2">
+      <c r="C49" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D49" s="2"/>
@@ -1809,14 +1834,14 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" ht="35.75" customHeight="1">
+    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D50" s="2"/>
@@ -1827,10 +1852,10 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" ht="35.75" customHeight="1">
+    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="2">
+      <c r="C51" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D51" s="2"/>
@@ -1841,10 +1866,10 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" ht="35.75" customHeight="1">
+    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
-      <c r="C52" s="2">
+      <c r="C52" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D52" s="2"/>
@@ -1855,14 +1880,14 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" ht="35.75" customHeight="1">
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D53" s="2"/>
@@ -1873,10 +1898,10 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" ht="35.75" customHeight="1">
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="2">
+      <c r="C54" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D54" s="2"/>
@@ -1887,14 +1912,14 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" ht="35.75" customHeight="1">
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D55" s="2"/>
@@ -1905,14 +1930,14 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" ht="35.75" customHeight="1">
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D56" s="2"/>
@@ -1923,14 +1948,14 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" ht="35.75" customHeight="1">
+    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D57" s="2"/>
@@ -1941,10 +1966,10 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" ht="35.75" customHeight="1">
+    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="2">
+      <c r="C58" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D58" s="2"/>
@@ -1955,14 +1980,14 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" ht="35.75" customHeight="1">
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D59" s="2"/>
@@ -1973,14 +1998,14 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" ht="35.75" customHeight="1">
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D60" s="2"/>
@@ -1991,14 +2016,14 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" ht="35.75" customHeight="1">
+    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D61" s="2"/>
@@ -2009,14 +2034,14 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" ht="35.75" customHeight="1">
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D62" s="2"/>
@@ -2027,14 +2052,14 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" ht="35.75" customHeight="1">
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D63" s="2"/>
@@ -2045,14 +2070,14 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" ht="35.75" customHeight="1">
+    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D64" s="2"/>
@@ -2063,14 +2088,14 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="35.75" customHeight="1">
+    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D65" s="2"/>
@@ -2081,14 +2106,14 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" ht="35.75" customHeight="1">
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D66" s="2"/>
@@ -2099,10 +2124,10 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" ht="35.75" customHeight="1">
+    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="2">
+      <c r="C67" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D67" s="2"/>
@@ -2113,14 +2138,14 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" ht="35.75" customHeight="1">
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D68" s="2"/>
@@ -2131,14 +2156,14 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" ht="35.75" customHeight="1">
+    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D69" s="2"/>
@@ -2149,14 +2174,14 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" ht="35.75" customHeight="1">
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D70" s="2"/>
@@ -2167,7 +2192,7 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" ht="35.75" customHeight="1">
+    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2179,17 +2204,17 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" ht="35.75" customHeight="1">
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="2">
-        <v>404</v>
-      </c>
-      <c r="D72" s="2">
+      <c r="C72" s="2" t="n">
+        <v>404</v>
+      </c>
+      <c r="D72" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E72" s="2"/>
@@ -2199,14 +2224,14 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" ht="35.75" customHeight="1">
+    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="2" t="n">
         <v>404</v>
       </c>
       <c r="D73" s="4"/>
@@ -2217,7 +2242,7 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" ht="35.75" customHeight="1">
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -2229,17 +2254,17 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" ht="35.75" customHeight="1">
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="2">
-        <v>404</v>
-      </c>
-      <c r="D75" s="2">
+      <c r="C75" s="2" t="n">
+        <v>404</v>
+      </c>
+      <c r="D75" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E75" s="2"/>
@@ -2249,7 +2274,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" ht="35.75" customHeight="1">
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2261,7 +2286,7 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" ht="35.75" customHeight="1">
+    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>59</v>
       </c>
@@ -2279,7 +2304,7 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" ht="35.75" customHeight="1">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
@@ -2298,16 +2323,16 @@
       <c r="J78" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B1:B36 B38:B40 B42:B70 B72:B73 B75:B1078" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B36 B38:B40 B42:B70 B72:B73 B75:B1078" type="list">
       <formula1>"store,restaurant,drink,entertainment,misc,coffee,snack"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2315,20 +2340,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="10" width="11.54296875" style="1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.75" customHeight="1">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2341,14 +2370,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="35.75" customHeight="1">
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2360,7 +2391,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="35.75" customHeight="1">
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2372,7 +2403,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="35.75" customHeight="1">
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2384,7 +2415,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="35.75" customHeight="1">
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2396,7 +2427,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="35.75" customHeight="1">
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2408,7 +2439,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="35.75" customHeight="1">
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>63</v>
       </c>
@@ -2426,7 +2457,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="35.75" customHeight="1">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2438,7 +2469,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="35.75" customHeight="1">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2450,7 +2481,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="35.75" customHeight="1">
+    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2462,7 +2493,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="35.75" customHeight="1">
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2474,7 +2505,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="35.75" customHeight="1">
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2486,7 +2517,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="35.75" customHeight="1">
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
@@ -2502,7 +2533,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="35.75" customHeight="1">
+    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>66</v>
       </c>
@@ -2518,7 +2549,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="35.75" customHeight="1">
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>67</v>
       </c>
@@ -2534,7 +2565,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="35.75" customHeight="1">
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2546,7 +2577,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="35.75" customHeight="1">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>68</v>
       </c>
@@ -2562,7 +2593,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="35.75" customHeight="1">
+    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2574,7 +2605,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="35.75" customHeight="1">
+    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2586,15 +2617,15 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="35.75" customHeight="1">
+    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2604,7 +2635,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="35.75" customHeight="1">
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2616,9 +2647,9 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="35.75" customHeight="1">
+    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>44</v>
@@ -2632,7 +2663,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="35.75" customHeight="1">
+    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2644,7 +2675,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="35.75" customHeight="1">
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2656,7 +2687,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="35.75" customHeight="1">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2668,7 +2699,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="35.75" customHeight="1">
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2680,7 +2711,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" ht="35.75" customHeight="1">
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2692,9 +2723,9 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="35.75" customHeight="1">
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>9</v>
@@ -2708,7 +2739,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="35.75" customHeight="1">
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2720,9 +2751,9 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" ht="35.75" customHeight="1">
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>44</v>
@@ -2736,7 +2767,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="35.75" customHeight="1">
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2748,7 +2779,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" ht="35.75" customHeight="1">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2760,7 +2791,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="35.75" customHeight="1">
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2772,7 +2803,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" ht="35.75" customHeight="1">
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2784,7 +2815,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" ht="35.75" customHeight="1">
+    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2796,7 +2827,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" ht="35.75" customHeight="1">
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2808,7 +2839,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="35.75" customHeight="1">
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2820,7 +2851,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="35.75" customHeight="1">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2832,7 +2863,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" ht="35.75" customHeight="1">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2844,7 +2875,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" ht="35.75" customHeight="1">
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2856,7 +2887,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="35.75" customHeight="1">
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2868,7 +2899,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" ht="35.75" customHeight="1">
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2880,7 +2911,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" ht="35.75" customHeight="1">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2892,7 +2923,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" ht="35.75" customHeight="1">
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2904,7 +2935,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" ht="35.75" customHeight="1">
+    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2916,7 +2947,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" ht="35.75" customHeight="1">
+    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2928,7 +2959,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" ht="35.75" customHeight="1">
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2940,7 +2971,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" ht="35.75" customHeight="1">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2952,9 +2983,9 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" ht="35.75" customHeight="1">
+    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>15</v>
@@ -2968,7 +2999,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" ht="35.75" customHeight="1">
+    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2980,7 +3011,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" ht="35.75" customHeight="1">
+    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2992,9 +3023,9 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" ht="35.75" customHeight="1">
+    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>9</v>
@@ -3008,7 +3039,7 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" ht="35.75" customHeight="1">
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -3020,9 +3051,9 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" ht="35.75" customHeight="1">
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>15</v>
@@ -3036,7 +3067,7 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" ht="35.75" customHeight="1">
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -3048,7 +3079,7 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" ht="35.75" customHeight="1">
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -3060,7 +3091,7 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" ht="35.75" customHeight="1">
+    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -3072,7 +3103,7 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" ht="35.75" customHeight="1">
+    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -3084,7 +3115,7 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" ht="35.75" customHeight="1">
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -3096,9 +3127,9 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" ht="35.75" customHeight="1">
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>44</v>
@@ -3112,7 +3143,7 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" ht="35.75" customHeight="1">
+    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -3124,7 +3155,7 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" ht="35.75" customHeight="1">
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -3136,9 +3167,9 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" ht="35.75" customHeight="1">
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>23</v>
@@ -3152,7 +3183,7 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" ht="35.75" customHeight="1">
+    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3164,7 +3195,7 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="35.75" customHeight="1">
+    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3176,9 +3207,9 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" ht="35.75" customHeight="1">
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>15</v>
@@ -3192,9 +3223,9 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" ht="35.75" customHeight="1">
+    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>35</v>
@@ -3208,7 +3239,7 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" ht="35.75" customHeight="1">
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3220,7 +3251,7 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" ht="35.75" customHeight="1">
+    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
         <v>53</v>
       </c>
@@ -3236,7 +3267,7 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" ht="35.75" customHeight="1">
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
         <v>55</v>
       </c>
@@ -3252,7 +3283,7 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" ht="35.75" customHeight="1">
+    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="2"/>
@@ -3264,15 +3295,15 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" ht="35.75" customHeight="1">
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C72" s="2"/>
-      <c r="D72" s="2">
+      <c r="D72" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E72" s="2"/>
@@ -3282,7 +3313,7 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" ht="35.75" customHeight="1">
+    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3294,7 +3325,7 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" ht="35.75" customHeight="1">
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3306,7 +3337,7 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" ht="35.75" customHeight="1">
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3318,7 +3349,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" ht="35.75" customHeight="1">
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3330,7 +3361,7 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" ht="35.75" customHeight="1">
+    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3342,7 +3373,7 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" ht="35.75" customHeight="1">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3355,16 +3386,16 @@
       <c r="J78" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B1:B70 B72:B1078" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B70 B72:B1078" type="list">
       <formula1>"store,restaurant,drink,entertainment,misc,coffee,snack"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
docs: Update bell_avenue and bell_suits
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ECC14A-C66B-4708-8D83-141C84812EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="1" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="G" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1'!$A$1:$E$1</definedName>
+  </definedNames>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -21,42 +29,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sitrus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sitrus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Flows Gourmet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restaurant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the-flows-gourmet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">蜀都风味</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Sitrus</t>
+  </si>
+  <si>
+    <t>sitrus</t>
+  </si>
+  <si>
+    <t>The Flows Gourmet</t>
+  </si>
+  <si>
+    <t>restaurant</t>
+  </si>
+  <si>
+    <t>the-flows-gourmet</t>
+  </si>
+  <si>
+    <t>蜀都风味</t>
   </si>
   <si>
     <r>
@@ -76,7 +81,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">闽桂中国超市</t>
+      <t>闽桂中国超市</t>
     </r>
   </si>
   <si>
@@ -97,7 +102,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">薯嘟嘟超市</t>
+      <t>薯嘟嘟超市</t>
     </r>
   </si>
   <si>
@@ -117,17 +122,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">车店</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">misc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DirectionsCarFilledRoundedIcon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Grind</t>
+      <t>车店</t>
+    </r>
+  </si>
+  <si>
+    <t>DirectionsCarFilledRoundedIcon</t>
+  </si>
+  <si>
+    <t>The Grind</t>
   </si>
   <si>
     <r>
@@ -147,7 +149,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">食坊</t>
+      <t>食坊</t>
     </r>
   </si>
   <si>
@@ -168,7 +170,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">礼品店</t>
+      <t>礼品店</t>
     </r>
   </si>
   <si>
@@ -189,17 +191,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">宠物诊所</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">KIMS SALON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starbucks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coffee</t>
+      <t>宠物诊所</t>
+    </r>
+  </si>
+  <si>
+    <t>KIMS SALON</t>
+  </si>
+  <si>
+    <t>Starbucks</t>
   </si>
   <si>
     <r>
@@ -219,7 +218,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">华莱士</t>
+      <t>华莱士</t>
     </r>
   </si>
   <si>
@@ -240,14 +239,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">蜜雪冰城</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">drink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KK</t>
+      <t>蜜雪冰城</t>
+    </r>
+  </si>
+  <si>
+    <t>KK</t>
   </si>
   <si>
     <r>
@@ -267,7 +263,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">冰雪时光</t>
+      <t>冰雪时光</t>
     </r>
   </si>
   <si>
@@ -291,7 +287,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">鸿运租车</t>
+      <t>鸿运租车</t>
     </r>
   </si>
   <si>
@@ -312,20 +308,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">新式快炒</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">沙县小吃</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PaoPaoPot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secret Recipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">snack</t>
+      <t>新式快炒</t>
+    </r>
+  </si>
+  <si>
+    <t>沙县小吃</t>
+  </si>
+  <si>
+    <t>PaoPaoPot</t>
+  </si>
+  <si>
+    <t>Secret Recipe</t>
+  </si>
+  <si>
+    <t>snack</t>
   </si>
   <si>
     <r>
@@ -345,7 +341,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">面对面</t>
+      <t>面对面</t>
     </r>
   </si>
   <si>
@@ -366,14 +362,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">麻辣诱惑</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">The Daily Kueh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">聚椒
+      <t>麻辣诱惑</t>
+    </r>
+  </si>
+  <si>
+    <t>The Daily Kueh</t>
+  </si>
+  <si>
+    <t>聚椒
 烤肉火锅店</t>
   </si>
   <si>
@@ -393,20 +389,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">甜点</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">洗衣房</t>
-  </si>
-  <si>
-    <t xml:space="preserve">申通快递</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black 8 Internatinoal Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entertainment</t>
+      <t>甜点</t>
+    </r>
+  </si>
+  <si>
+    <t>洗衣房</t>
+  </si>
+  <si>
+    <t>申通快递</t>
+  </si>
+  <si>
+    <t>Black 8 Internatinoal Club</t>
+  </si>
+  <si>
+    <t>entertainment</t>
   </si>
   <si>
     <r>
@@ -426,7 +422,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">ZEKUN TCM HEALTHCARE</t>
+      <t>ZEKUN TCM HEALTHCARE</t>
     </r>
   </si>
   <si>
@@ -447,17 +443,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Xinjiang Restaurant</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Event Space</t>
-  </si>
-  <si>
-    <t xml:space="preserve">百家牛肉面</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baskin Robbins BR</t>
+      <t>Xinjiang Restaurant</t>
+    </r>
+  </si>
+  <si>
+    <t>Event Space</t>
+  </si>
+  <si>
+    <t>百家牛肉面</t>
+  </si>
+  <si>
+    <t>Baskin Robbins BR</t>
   </si>
   <si>
     <r>
@@ -477,7 +473,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">冰室</t>
+      <t>冰室</t>
     </r>
   </si>
   <si>
@@ -498,29 +494,29 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">ChaPanda</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">大圣烧烤</t>
-  </si>
-  <si>
-    <t xml:space="preserve">金龙牛肉煲仔饭</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vape Coffee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">鸡公煲</t>
-  </si>
-  <si>
-    <t xml:space="preserve">笆篱是家大排档</t>
-  </si>
-  <si>
-    <t xml:space="preserve">茶作饮品店</t>
-  </si>
-  <si>
-    <t xml:space="preserve">佳粤</t>
+      <t>ChaPanda</t>
+    </r>
+  </si>
+  <si>
+    <t>大圣烧烤</t>
+  </si>
+  <si>
+    <t>金龙牛肉煲仔饭</t>
+  </si>
+  <si>
+    <t>Vape Coffee</t>
+  </si>
+  <si>
+    <t>鸡公煲</t>
+  </si>
+  <si>
+    <t>笆篱是家大排档</t>
+  </si>
+  <si>
+    <t>茶作饮品店</t>
+  </si>
+  <si>
+    <t>佳粤</t>
   </si>
   <si>
     <r>
@@ -540,30 +536,30 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">一二爽便利咖</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">123express-mart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nasi Kandar Mamak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mamak</t>
+      <t>一二爽便利咖</t>
+    </r>
+  </si>
+  <si>
+    <t>123express-mart</t>
+  </si>
+  <si>
+    <t>Nasi Kandar Mamak</t>
+  </si>
+  <si>
+    <t>mamak</t>
   </si>
   <si>
     <t xml:space="preserve">ChaZhuGong Milk tea
 </t>
   </si>
   <si>
-    <t xml:space="preserve">chazhugong-milk-tea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cafe Lazatnyo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gepreking Fried Kitchen</t>
+    <t>chazhugong-milk-tea</t>
+  </si>
+  <si>
+    <t>Cafe Lazatnyo</t>
+  </si>
+  <si>
+    <t>Gepreking Fried Kitchen</t>
   </si>
   <si>
     <r>
@@ -583,17 +579,17 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Stella Vet</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">CHATTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marqa Caff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marqacaff</t>
+      <t>Stella Vet</t>
+    </r>
+  </si>
+  <si>
+    <t>CHATTO</t>
+  </si>
+  <si>
+    <t>Marqa Caff</t>
+  </si>
+  <si>
+    <t>marqacaff</t>
   </si>
   <si>
     <r>
@@ -613,7 +609,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Yoga</t>
+      <t>Yoga</t>
     </r>
   </si>
   <si>
@@ -634,11 +630,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Braised Chicken</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Real Peak Music</t>
+      <t>Braised Chicken</t>
+    </r>
+  </si>
+  <si>
+    <t>Real Peak Music</t>
   </si>
   <si>
     <r>
@@ -658,7 +654,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">People’s Bookstore</t>
+      <t>People’s Bookstore</t>
     </r>
   </si>
   <si>
@@ -679,7 +675,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Grilled Fish</t>
+      <t>Grilled Fish</t>
     </r>
   </si>
   <si>
@@ -700,7 +696,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Real Estate</t>
+      <t>Real Estate</t>
     </r>
   </si>
   <si>
@@ -720,11 +716,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">桌游店</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SENZE CAFE</t>
+      <t>桌游店</t>
+    </r>
+  </si>
+  <si>
+    <t>SENZE CAFE</t>
   </si>
   <si>
     <r>
@@ -744,7 +740,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Korean Speaking Class</t>
+      <t>Korean Speaking Class</t>
     </r>
   </si>
   <si>
@@ -765,7 +761,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">XILE DESSERT</t>
+      <t>XILE DESSERT</t>
     </r>
   </si>
   <si>
@@ -786,18 +782,21 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Billiard Hall</t>
-    </r>
+      <t>Billiard Hall</t>
+    </r>
+  </si>
+  <si>
+    <t>daily_necessity</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -806,24 +805,15 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="LXGW WenKai Mono"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -835,130 +825,112 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -1011,28 +983,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C78" activeCellId="0" sqref="C78"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.54"/>
+    <col min="1" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="35.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1054,15 +1024,15 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="35.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1072,15 +1042,15 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" ht="35.25" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1090,10 +1060,10 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" ht="35.25" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>404</v>
       </c>
       <c r="D4" s="2"/>
@@ -1104,10 +1074,10 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="35.25" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>404</v>
       </c>
       <c r="D5" s="2"/>
@@ -1118,14 +1088,14 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" ht="35.25" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
         <v>404</v>
       </c>
       <c r="D6" s="2"/>
@@ -1136,14 +1106,14 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" ht="35.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C7" s="2">
         <v>404</v>
       </c>
       <c r="D7" s="2"/>
@@ -1154,14 +1124,14 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" ht="35.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C8" s="2">
         <v>404</v>
       </c>
       <c r="D8" s="2"/>
@@ -1172,21 +1142,21 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" ht="35.25" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="2">
+        <v>404</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>404</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1194,10 +1164,10 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" ht="35.25" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="2">
         <v>404</v>
       </c>
       <c r="D10" s="2"/>
@@ -1208,14 +1178,14 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" ht="35.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
         <v>404</v>
       </c>
       <c r="D11" s="2"/>
@@ -1226,14 +1196,14 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" ht="35.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
         <v>404</v>
       </c>
       <c r="D12" s="2"/>
@@ -1244,14 +1214,14 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" ht="35.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2">
         <v>404</v>
       </c>
       <c r="D13" s="2"/>
@@ -1262,10 +1232,10 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" ht="35.25" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="2">
         <v>404</v>
       </c>
       <c r="D14" s="2"/>
@@ -1276,14 +1246,14 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" ht="35.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C15" s="2">
         <v>404</v>
       </c>
       <c r="D15" s="2"/>
@@ -1294,14 +1264,14 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+    <row r="16" spans="1:10" ht="35.25" customHeight="1">
+      <c r="A16" s="2">
         <v>711</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C16" s="2">
         <v>404</v>
       </c>
       <c r="D16" s="2"/>
@@ -1312,14 +1282,14 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" ht="35.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C17" s="2">
         <v>404</v>
       </c>
       <c r="D17" s="2"/>
@@ -1330,10 +1300,10 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" ht="35.25" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="2">
         <v>404</v>
       </c>
       <c r="D18" s="2"/>
@@ -1344,10 +1314,10 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" ht="35.25" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="2">
         <v>404</v>
       </c>
       <c r="D19" s="2"/>
@@ -1358,14 +1328,14 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" ht="35.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2">
         <v>404</v>
       </c>
       <c r="D20" s="2"/>
@@ -1376,14 +1346,14 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10" ht="35.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2">
         <v>404</v>
       </c>
       <c r="D21" s="2"/>
@@ -1394,14 +1364,14 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10" ht="35.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C22" s="2">
         <v>404</v>
       </c>
       <c r="D22" s="2"/>
@@ -1412,10 +1382,10 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" ht="35.25" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="2">
         <v>404</v>
       </c>
       <c r="D23" s="2"/>
@@ -1426,14 +1396,14 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" ht="35.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C24" s="2">
         <v>404</v>
       </c>
       <c r="D24" s="2"/>
@@ -1444,10 +1414,10 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" ht="35.25" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2" t="n">
+      <c r="C25" s="2">
         <v>404</v>
       </c>
       <c r="D25" s="2"/>
@@ -1458,14 +1428,14 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" ht="35.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C26" s="2">
         <v>404</v>
       </c>
       <c r="D26" s="2"/>
@@ -1476,10 +1446,10 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10" ht="35.25" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2" t="n">
+      <c r="C27" s="2">
         <v>404</v>
       </c>
       <c r="D27" s="2"/>
@@ -1490,14 +1460,14 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10" ht="35.25" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2">
         <v>404</v>
       </c>
       <c r="D28" s="2"/>
@@ -1508,14 +1478,14 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" ht="35.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="C29" s="2">
         <v>404</v>
       </c>
       <c r="D29" s="2"/>
@@ -1526,14 +1496,14 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" ht="35.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C30" s="2">
         <v>404</v>
       </c>
       <c r="D30" s="2"/>
@@ -1544,14 +1514,14 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" ht="35.25" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2">
         <v>404</v>
       </c>
       <c r="D31" s="2"/>
@@ -1562,14 +1532,14 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10" ht="35.25" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C32" s="2">
         <v>404</v>
       </c>
       <c r="D32" s="2"/>
@@ -1580,14 +1550,14 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" ht="35.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C33" s="2">
         <v>404</v>
       </c>
       <c r="D33" s="2"/>
@@ -1598,10 +1568,10 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10" ht="35.25" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2" t="n">
+      <c r="C34" s="2">
         <v>404</v>
       </c>
       <c r="D34" s="2"/>
@@ -1612,10 +1582,10 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" ht="35.25" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="2" t="n">
+      <c r="C35" s="2">
         <v>404</v>
       </c>
       <c r="D35" s="2"/>
@@ -1626,14 +1596,14 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" ht="35.25" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2">
         <v>404</v>
       </c>
       <c r="D36" s="2"/>
@@ -1644,10 +1614,10 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10" ht="35.25" customHeight="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="2" t="n">
+      <c r="C37" s="2">
         <v>404</v>
       </c>
       <c r="D37" s="2"/>
@@ -1658,14 +1628,14 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10" ht="35.25" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2">
         <v>404</v>
       </c>
       <c r="D38" s="2"/>
@@ -1676,14 +1646,14 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10" ht="35.25" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C39" s="2">
         <v>404</v>
       </c>
       <c r="D39" s="2"/>
@@ -1694,10 +1664,10 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10" ht="35.25" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="2" t="n">
+      <c r="C40" s="2">
         <v>404</v>
       </c>
       <c r="D40" s="2"/>
@@ -1708,10 +1678,10 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10" ht="35.25" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="2" t="n">
+      <c r="C41" s="2">
         <v>404</v>
       </c>
       <c r="D41" s="2"/>
@@ -1722,10 +1692,10 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:10" ht="35.25" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="2" t="n">
+      <c r="C42" s="2">
         <v>404</v>
       </c>
       <c r="D42" s="2"/>
@@ -1736,10 +1706,10 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10" ht="35.25" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="2">
         <v>404</v>
       </c>
       <c r="D43" s="2"/>
@@ -1750,10 +1720,10 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:10" ht="35.25" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="2">
         <v>404</v>
       </c>
       <c r="D44" s="2"/>
@@ -1764,10 +1734,10 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:10" ht="35.25" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2" t="n">
+      <c r="C45" s="2">
         <v>404</v>
       </c>
       <c r="D45" s="2"/>
@@ -1778,10 +1748,10 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:10" ht="35.25" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="2" t="n">
+      <c r="C46" s="2">
         <v>404</v>
       </c>
       <c r="D46" s="2"/>
@@ -1792,10 +1762,10 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:10" ht="35.25" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="2" t="n">
+      <c r="C47" s="2">
         <v>404</v>
       </c>
       <c r="D47" s="2"/>
@@ -1806,10 +1776,10 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:10" ht="35.25" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="2" t="n">
+      <c r="C48" s="2">
         <v>404</v>
       </c>
       <c r="D48" s="2"/>
@@ -1820,10 +1790,10 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:10" ht="35.25" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="2" t="n">
+      <c r="C49" s="2">
         <v>404</v>
       </c>
       <c r="D49" s="2"/>
@@ -1834,14 +1804,14 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:10" ht="35.25" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C50" s="2">
         <v>404</v>
       </c>
       <c r="D50" s="2"/>
@@ -1852,10 +1822,10 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:10" ht="35.25" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="2" t="n">
+      <c r="C51" s="2">
         <v>404</v>
       </c>
       <c r="D51" s="2"/>
@@ -1866,10 +1836,10 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:10" ht="35.25" customHeight="1">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
-      <c r="C52" s="2" t="n">
+      <c r="C52" s="2">
         <v>404</v>
       </c>
       <c r="D52" s="2"/>
@@ -1880,14 +1850,14 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:10" ht="35.25" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C53" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C53" s="2">
         <v>404</v>
       </c>
       <c r="D53" s="2"/>
@@ -1898,10 +1868,10 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:10" ht="35.25" customHeight="1">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="2" t="n">
+      <c r="C54" s="2">
         <v>404</v>
       </c>
       <c r="D54" s="2"/>
@@ -1912,14 +1882,14 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:10" ht="35.25" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C55" s="2">
         <v>404</v>
       </c>
       <c r="D55" s="2"/>
@@ -1930,14 +1900,14 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:10" ht="35.25" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C56" s="2">
         <v>404</v>
       </c>
       <c r="D56" s="2"/>
@@ -1948,14 +1918,14 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:10" ht="35.25" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C57" s="2">
         <v>404</v>
       </c>
       <c r="D57" s="2"/>
@@ -1966,10 +1936,10 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:10" ht="35.25" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="2" t="n">
+      <c r="C58" s="2">
         <v>404</v>
       </c>
       <c r="D58" s="2"/>
@@ -1980,14 +1950,14 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:10" ht="35.25" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C59" s="2">
         <v>404</v>
       </c>
       <c r="D59" s="2"/>
@@ -1998,14 +1968,14 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:10" ht="35.25" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C60" s="2">
         <v>404</v>
       </c>
       <c r="D60" s="2"/>
@@ -2016,14 +1986,14 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:10" ht="35.25" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C61" s="2">
         <v>404</v>
       </c>
       <c r="D61" s="2"/>
@@ -2034,14 +2004,14 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:10" ht="35.25" customHeight="1">
       <c r="A62" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C62" s="2">
         <v>404</v>
       </c>
       <c r="D62" s="2"/>
@@ -2052,14 +2022,14 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:10" ht="35.25" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C63" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C63" s="2">
         <v>404</v>
       </c>
       <c r="D63" s="2"/>
@@ -2070,14 +2040,14 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:10" ht="35.25" customHeight="1">
       <c r="A64" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C64" s="2">
         <v>404</v>
       </c>
       <c r="D64" s="2"/>
@@ -2088,14 +2058,14 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:10" ht="35.25" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C65" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C65" s="2">
         <v>404</v>
       </c>
       <c r="D65" s="2"/>
@@ -2106,14 +2076,14 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:10" ht="35.25" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C66" s="2">
         <v>404</v>
       </c>
       <c r="D66" s="2"/>
@@ -2124,10 +2094,10 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:10" ht="35.25" customHeight="1">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="2" t="n">
+      <c r="C67" s="2">
         <v>404</v>
       </c>
       <c r="D67" s="2"/>
@@ -2138,14 +2108,14 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:10" ht="35.25" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C68" s="2">
         <v>404</v>
       </c>
       <c r="D68" s="2"/>
@@ -2156,14 +2126,14 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:10" ht="35.25" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C69" s="2">
         <v>404</v>
       </c>
       <c r="D69" s="2"/>
@@ -2174,14 +2144,14 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:10" ht="35.25" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C70" s="2">
         <v>404</v>
       </c>
       <c r="D70" s="2"/>
@@ -2192,7 +2162,7 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:10" ht="35.25" customHeight="1">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2204,17 +2174,17 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:10" ht="35.25" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" s="2" t="n">
-        <v>404</v>
-      </c>
-      <c r="D72" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C72" s="2">
+        <v>404</v>
+      </c>
+      <c r="D72" s="2">
         <v>2</v>
       </c>
       <c r="E72" s="2"/>
@@ -2224,14 +2194,14 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:10" ht="35.25" customHeight="1">
       <c r="A73" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C73" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C73" s="2">
         <v>404</v>
       </c>
       <c r="D73" s="4"/>
@@ -2242,7 +2212,7 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:10" ht="35.25" customHeight="1">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -2254,17 +2224,17 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:10" ht="35.25" customHeight="1">
       <c r="A75" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" s="2" t="n">
-        <v>404</v>
-      </c>
-      <c r="D75" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C75" s="2">
+        <v>404</v>
+      </c>
+      <c r="D75" s="2">
         <v>2</v>
       </c>
       <c r="E75" s="2"/>
@@ -2274,7 +2244,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:10" ht="35.25" customHeight="1">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2286,15 +2256,15 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:10" ht="35.25" customHeight="1">
       <c r="A77" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -2304,15 +2274,15 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:10" ht="35.25" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -2323,16 +2293,15 @@
       <c r="J78" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B36 B38:B40 B42:B70 B72:B73 B75:B1078" type="list">
-      <formula1>"store,restaurant,drink,entertainment,misc,coffee,snack"</formula1>
-      <formula2>0</formula2>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{D9F78479-56F5-4324-9BD7-3C4E3B68CA8C}">
+      <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2340,24 +2309,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="11.54"/>
+    <col min="1" max="10" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="35.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2379,7 +2344,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="35.25" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2391,7 +2356,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" ht="35.25" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2403,7 +2368,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" ht="35.25" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2415,7 +2380,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="35.25" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2427,7 +2392,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" ht="35.25" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2439,15 +2404,15 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" ht="35.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2457,7 +2422,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" ht="35.25" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2469,7 +2434,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" ht="35.25" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2481,7 +2446,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" ht="35.25" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2493,7 +2458,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" ht="35.25" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2505,7 +2470,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" ht="35.25" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2517,12 +2482,12 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" ht="35.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2533,12 +2498,12 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" ht="35.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2549,12 +2514,12 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" ht="35.25" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2565,7 +2530,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10" ht="35.25" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2577,12 +2542,12 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" ht="35.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2593,7 +2558,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" ht="35.25" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2605,7 +2570,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" ht="35.25" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2617,15 +2582,15 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" ht="35.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2635,7 +2600,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10" ht="35.25" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2647,12 +2612,12 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10" ht="35.25" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2663,7 +2628,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" ht="35.25" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2675,7 +2640,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" ht="35.25" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2687,7 +2652,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" ht="35.25" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2699,7 +2664,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" ht="35.25" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2711,7 +2676,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10" ht="35.25" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2723,12 +2688,12 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10" ht="35.25" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2739,7 +2704,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" ht="35.25" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2751,12 +2716,12 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" ht="35.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2767,7 +2732,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" ht="35.25" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2779,7 +2744,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10" ht="35.25" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2791,7 +2756,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" ht="35.25" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2803,7 +2768,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10" ht="35.25" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2815,7 +2780,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" ht="35.25" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2827,7 +2792,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" ht="35.25" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2839,7 +2804,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10" ht="35.25" customHeight="1">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2851,7 +2816,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10" ht="35.25" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2863,7 +2828,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10" ht="35.25" customHeight="1">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2875,7 +2840,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10" ht="35.25" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2887,7 +2852,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10" ht="35.25" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2899,7 +2864,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:10" ht="35.25" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2911,7 +2876,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10" ht="35.25" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2923,7 +2888,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:10" ht="35.25" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2935,7 +2900,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:10" ht="35.25" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2947,7 +2912,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:10" ht="35.25" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2959,7 +2924,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:10" ht="35.25" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2971,7 +2936,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:10" ht="35.25" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2983,12 +2948,12 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:10" ht="35.25" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2999,7 +2964,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:10" ht="35.25" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3011,7 +2976,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:10" ht="35.25" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3023,12 +2988,12 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:10" ht="35.25" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -3039,7 +3004,7 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:10" ht="35.25" customHeight="1">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -3051,12 +3016,12 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:10" ht="35.25" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -3067,7 +3032,7 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:10" ht="35.25" customHeight="1">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -3079,7 +3044,7 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:10" ht="35.25" customHeight="1">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -3091,7 +3056,7 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:10" ht="35.25" customHeight="1">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -3103,7 +3068,7 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:10" ht="35.25" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -3115,7 +3080,7 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:10" ht="35.25" customHeight="1">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -3127,12 +3092,12 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:10" ht="35.25" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -3143,7 +3108,7 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:10" ht="35.25" customHeight="1">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -3155,7 +3120,7 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:10" ht="35.25" customHeight="1">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -3167,12 +3132,12 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:10" ht="35.25" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3183,7 +3148,7 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:10" ht="35.25" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3195,7 +3160,7 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:10" ht="35.25" customHeight="1">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3207,12 +3172,12 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:10" ht="35.25" customHeight="1">
       <c r="A66" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -3223,12 +3188,12 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:10" ht="35.25" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -3239,7 +3204,7 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:10" ht="35.25" customHeight="1">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3251,12 +3216,12 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:10" ht="35.25" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -3267,12 +3232,12 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:10" ht="35.25" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -3283,7 +3248,7 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:10" ht="35.25" customHeight="1">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="2"/>
@@ -3295,15 +3260,15 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:10" ht="35.25" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C72" s="2"/>
-      <c r="D72" s="2" t="n">
+      <c r="D72" s="2">
         <v>2</v>
       </c>
       <c r="E72" s="2"/>
@@ -3313,7 +3278,7 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:10" ht="35.25" customHeight="1">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3325,7 +3290,7 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:10" ht="35.25" customHeight="1">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3337,7 +3302,7 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:10" ht="35.25" customHeight="1">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3349,7 +3314,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:10" ht="35.25" customHeight="1">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3361,7 +3326,7 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:10" ht="35.25" customHeight="1">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3373,7 +3338,7 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:10" ht="35.25" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3386,16 +3351,15 @@
       <c r="J78" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B70 B72:B1078" type="list">
-      <formula1>"store,restaurant,drink,entertainment,misc,coffee,snack"</formula1>
-      <formula2>0</formula2>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{D9E3693E-53AA-4983-A999-03CE3ACB1409}">
+      <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
docs: update bell_avenue and bell_suite
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ECC14A-C66B-4708-8D83-141C84812EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60664CE3-0B3B-4F78-ABF0-5632B2483AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1'!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -790,6 +790,10 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>xiledessert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2313,8 +2317,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -3195,7 +3199,9 @@
       <c r="B67" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C67" s="2"/>
+      <c r="C67" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>

</xml_diff>

<commit_message>
docs: update bell_avenue slug
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60664CE3-0B3B-4F78-ABF0-5632B2483AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C205839-70CA-49A6-BD18-FF485D5AE48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="G" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -426,6 +426,25 @@
     </r>
   </si>
   <si>
+    <t>Event Space</t>
+  </si>
+  <si>
+    <t>百家牛肉面</t>
+  </si>
+  <si>
+    <t>Baskin Robbins BR</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">R.W F&amp;B
+</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -433,6 +452,327 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t>冰室</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">茶百道
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ChaPanda</t>
+    </r>
+  </si>
+  <si>
+    <t>大圣烧烤</t>
+  </si>
+  <si>
+    <t>金龙牛肉煲仔饭</t>
+  </si>
+  <si>
+    <t>Vape Coffee</t>
+  </si>
+  <si>
+    <t>鸡公煲</t>
+  </si>
+  <si>
+    <t>笆篱是家大排档</t>
+  </si>
+  <si>
+    <t>茶作饮品店</t>
+  </si>
+  <si>
+    <t>佳粤</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">123ExpressMart
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>一二爽便利咖</t>
+    </r>
+  </si>
+  <si>
+    <t>123express-mart</t>
+  </si>
+  <si>
+    <t>Nasi Kandar Mamak</t>
+  </si>
+  <si>
+    <t>mamak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChaZhuGong Milk tea
+</t>
+  </si>
+  <si>
+    <t>chazhugong-milk-tea</t>
+  </si>
+  <si>
+    <t>Cafe Lazatnyo</t>
+  </si>
+  <si>
+    <t>Gepreking Fried Kitchen</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">宠物杂货店
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Stella Vet</t>
+    </r>
+  </si>
+  <si>
+    <t>CHATTO</t>
+  </si>
+  <si>
+    <t>Marqa Caff</t>
+  </si>
+  <si>
+    <t>marqacaff</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">瑜伽
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Yoga</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">黄焖鸡
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Braised Chicken</t>
+    </r>
+  </si>
+  <si>
+    <t>Real Peak Music</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">人民书局
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>People’s Bookstore</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">烤鱼
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Grilled Fish</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">房地产
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Real Estate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sword </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>桌游店</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">韩语口语班
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Korean Speaking Class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">喜乐冰铺
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>XILE DESSERT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">台球厅
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Billiard Hall</t>
+    </r>
+  </si>
+  <si>
+    <t>daily_necessity</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>xiledessert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">新疆餐厅
 </t>
     </r>
@@ -445,354 +785,21 @@
       </rPr>
       <t>Xinjiang Restaurant</t>
     </r>
-  </si>
-  <si>
-    <t>Event Space</t>
-  </si>
-  <si>
-    <t>百家牛肉面</t>
-  </si>
-  <si>
-    <t>Baskin Robbins BR</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R.W F&amp;B
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>冰室</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">茶百道
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ChaPanda</t>
-    </r>
-  </si>
-  <si>
-    <t>大圣烧烤</t>
-  </si>
-  <si>
-    <t>金龙牛肉煲仔饭</t>
-  </si>
-  <si>
-    <t>Vape Coffee</t>
-  </si>
-  <si>
-    <t>鸡公煲</t>
-  </si>
-  <si>
-    <t>笆篱是家大排档</t>
-  </si>
-  <si>
-    <t>茶作饮品店</t>
-  </si>
-  <si>
-    <t>佳粤</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">123ExpressMart
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>一二爽便利咖</t>
-    </r>
-  </si>
-  <si>
-    <t>123express-mart</t>
-  </si>
-  <si>
-    <t>Nasi Kandar Mamak</t>
-  </si>
-  <si>
-    <t>mamak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChaZhuGong Milk tea
-</t>
-  </si>
-  <si>
-    <t>chazhugong-milk-tea</t>
-  </si>
-  <si>
-    <t>Cafe Lazatnyo</t>
-  </si>
-  <si>
-    <t>Gepreking Fried Kitchen</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">宠物杂货店
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Stella Vet</t>
-    </r>
-  </si>
-  <si>
-    <t>CHATTO</t>
-  </si>
-  <si>
-    <t>Marqa Caff</t>
-  </si>
-  <si>
-    <t>marqacaff</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">瑜伽
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Yoga</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">黄焖鸡
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Braised Chicken</t>
-    </r>
-  </si>
-  <si>
-    <t>Real Peak Music</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">人民书局
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>People’s Bookstore</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">烤鱼
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Grilled Fish</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">房地产
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Real Estate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Sword </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>桌游店</t>
-    </r>
-  </si>
-  <si>
-    <t>SENZE CAFE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">韩语口语班
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Korean Speaking Class</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">喜乐冰铺
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>XILE DESSERT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">台球厅
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Billiard Hall</t>
-    </r>
-  </si>
-  <si>
-    <t>daily_necessity</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>xiledessert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xinjiang-Restaurant</t>
+  </si>
+  <si>
+    <t>SENZE CAFF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sword</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>senzecaff</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -996,9 +1003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1033,7 +1040,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -1115,7 +1122,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="2">
         <v>404</v>
@@ -1133,7 +1140,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2">
         <v>404</v>
@@ -1151,7 +1158,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2">
         <v>404</v>
@@ -1255,7 +1262,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="2">
         <v>404</v>
@@ -1273,7 +1280,7 @@
         <v>711</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C16" s="2">
         <v>404</v>
@@ -1291,7 +1298,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" s="2">
         <v>404</v>
@@ -1405,7 +1412,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2">
         <v>404</v>
@@ -1487,7 +1494,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C29" s="2">
         <v>404</v>
@@ -1891,7 +1898,7 @@
         <v>37</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C55" s="2">
         <v>404</v>
@@ -1909,7 +1916,7 @@
         <v>38</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C56" s="2">
         <v>404</v>
@@ -1959,7 +1966,7 @@
         <v>41</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C59" s="2">
         <v>404</v>
@@ -1974,13 +1981,13 @@
     </row>
     <row r="60" spans="1:10" ht="35.25" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="2">
-        <v>404</v>
+      <c r="C60" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1992,7 +1999,7 @@
     </row>
     <row r="61" spans="1:10" ht="35.25" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>40</v>
@@ -2010,7 +2017,7 @@
     </row>
     <row r="62" spans="1:10" ht="35.25" customHeight="1">
       <c r="A62" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>8</v>
@@ -2028,7 +2035,7 @@
     </row>
     <row r="63" spans="1:10" ht="35.25" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>31</v>
@@ -2046,7 +2053,7 @@
     </row>
     <row r="64" spans="1:10" ht="35.25" customHeight="1">
       <c r="A64" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>8</v>
@@ -2064,7 +2071,7 @@
     </row>
     <row r="65" spans="1:10" ht="35.25" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>31</v>
@@ -2082,7 +2089,7 @@
     </row>
     <row r="66" spans="1:10" ht="35.25" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>8</v>
@@ -2114,7 +2121,7 @@
     </row>
     <row r="68" spans="1:10" ht="35.25" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>8</v>
@@ -2132,7 +2139,7 @@
     </row>
     <row r="69" spans="1:10" ht="35.25" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>31</v>
@@ -2150,7 +2157,7 @@
     </row>
     <row r="70" spans="1:10" ht="35.25" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>8</v>
@@ -2180,7 +2187,7 @@
     </row>
     <row r="72" spans="1:10" ht="35.25" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>8</v>
@@ -2200,7 +2207,7 @@
     </row>
     <row r="73" spans="1:10" ht="35.25" customHeight="1">
       <c r="A73" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>31</v>
@@ -2230,7 +2237,7 @@
     </row>
     <row r="75" spans="1:10" ht="35.25" customHeight="1">
       <c r="A75" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>8</v>
@@ -2262,13 +2269,13 @@
     </row>
     <row r="77" spans="1:10" ht="35.25" customHeight="1">
       <c r="A77" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -2280,13 +2287,13 @@
     </row>
     <row r="78" spans="1:10" ht="35.25" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -2316,9 +2323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -2410,13 +2417,13 @@
     </row>
     <row r="7" spans="1:10" ht="35.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2488,7 +2495,7 @@
     </row>
     <row r="13" spans="1:10" ht="35.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>31</v>
@@ -2504,7 +2511,7 @@
     </row>
     <row r="14" spans="1:10" ht="35.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -2520,10 +2527,10 @@
     </row>
     <row r="15" spans="1:10" ht="35.25" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2548,7 +2555,7 @@
     </row>
     <row r="17" spans="1:10" ht="35.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -2588,13 +2595,13 @@
     </row>
     <row r="20" spans="1:10" ht="35.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2618,7 +2625,7 @@
     </row>
     <row r="22" spans="1:10" ht="35.25" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>40</v>
@@ -2694,7 +2701,7 @@
     </row>
     <row r="28" spans="1:10" ht="35.25" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
@@ -2722,7 +2729,7 @@
     </row>
     <row r="30" spans="1:10" ht="35.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>40</v>
@@ -2954,10 +2961,10 @@
     </row>
     <row r="49" spans="1:10" ht="35.25" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2994,7 +3001,7 @@
     </row>
     <row r="52" spans="1:10" ht="35.25" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>8</v>
@@ -3022,10 +3029,10 @@
     </row>
     <row r="54" spans="1:10" ht="35.25" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -3098,12 +3105,14 @@
     </row>
     <row r="60" spans="1:10" ht="35.25" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C60" s="2"/>
+      <c r="C60" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -3138,12 +3147,14 @@
     </row>
     <row r="63" spans="1:10" ht="35.25" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -3178,10 +3189,10 @@
     </row>
     <row r="66" spans="1:10" ht="35.25" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -3194,13 +3205,13 @@
     </row>
     <row r="67" spans="1:10" ht="35.25" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -3224,7 +3235,7 @@
     </row>
     <row r="69" spans="1:10" ht="35.25" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>8</v>
@@ -3240,7 +3251,7 @@
     </row>
     <row r="70" spans="1:10" ht="35.25" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>8</v>
@@ -3268,7 +3279,7 @@
     </row>
     <row r="72" spans="1:10" ht="35.25" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
docs: Add eathami and 369express post
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C205839-70CA-49A6-BD18-FF485D5AE48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48177445-8180-4E79-89DF-745840709A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -800,6 +800,14 @@
   </si>
   <si>
     <t>senzecaff</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>369express</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>eathami</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1004,8 +1012,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1214,8 +1222,8 @@
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2">
-        <v>404</v>
+      <c r="C12" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1514,8 +1522,8 @@
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="2">
-        <v>404</v>
+      <c r="C30" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>

</xml_diff>

<commit_message>
feat: update bell_avenue and fix map-lack klinik
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48177445-8180-4E79-89DF-745840709A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BED5992-9415-4724-A88E-13D9AD37C664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -808,6 +808,29 @@
   </si>
   <si>
     <t>eathami</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>heystationery</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Klinik Cosmomedic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>诊所</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>klinik</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -815,7 +838,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -832,6 +855,12 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -870,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -882,6 +911,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1012,8 +1045,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1240,8 +1273,8 @@
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="2">
-        <v>404</v>
+      <c r="C13" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1498,14 +1531,14 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="2">
-        <v>404</v>
+      <c r="A29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1517,13 +1550,13 @@
     </row>
     <row r="30" spans="1:10" ht="35.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
+      </c>
+      <c r="C30" s="2">
+        <v>404</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1534,14 +1567,14 @@
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A31" s="3" t="s">
-        <v>28</v>
+      <c r="A31" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="2">
-        <v>404</v>
+      <c r="C31" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1552,8 +1585,8 @@
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>29</v>
+      <c r="A32" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>8</v>
@@ -1571,10 +1604,10 @@
     </row>
     <row r="33" spans="1:10" ht="35.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C33" s="2">
         <v>404</v>
@@ -1588,8 +1621,12 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C34" s="2">
         <v>404</v>
       </c>
@@ -1634,8 +1671,8 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="2">
         <v>404</v>
       </c>

</xml_diff>

<commit_message>
feat: Update bell_avenue with spicytemptation
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BED5992-9415-4724-A88E-13D9AD37C664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A354F684-9037-44A3-A5D4-3E4C6D4C545A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="2090" windowWidth="19200" windowHeight="10790" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="G" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -831,6 +831,10 @@
   </si>
   <si>
     <t>klinik</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>spicytemtation</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1045,8 +1049,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1691,8 +1695,8 @@
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="2">
-        <v>404</v>
+      <c r="C38" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>

</xml_diff>

<commit_message>
fix: fix bell_avenue with spicytemptation
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEA0301-DC77-42CC-A12F-797A19A74500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D860C29-8A26-4509-8390-F729FA9E9A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4050" yWindow="2090" windowWidth="19200" windowHeight="10790" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -810,10 +810,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>spicytemtation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">369 Express
 </t>
@@ -835,6 +831,10 @@
   </si>
   <si>
     <t>shaxian</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>spicytemptation</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1049,8 +1049,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="31" spans="1:10" ht="35.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>8</v>
@@ -1590,13 +1590,13 @@
     </row>
     <row r="32" spans="1:10" ht="35.25" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1696,7 +1696,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>

</xml_diff>

<commit_message>
docs: Add 711, kk, kimssalon posts
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D860C29-8A26-4509-8390-F729FA9E9A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC5132F-A9A9-40D4-83CA-56580414F5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4050" yWindow="2090" windowWidth="19200" windowHeight="10790" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -835,6 +835,14 @@
   </si>
   <si>
     <t>spicytemptation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>kimssalon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>kk</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1049,8 +1057,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N34" sqref="N34"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1328,7 +1336,7 @@
         <v>74</v>
       </c>
       <c r="C16" s="2">
-        <v>404</v>
+        <v>711</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1345,8 +1353,8 @@
       <c r="B17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="2">
-        <v>404</v>
+      <c r="C17" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1459,8 +1467,8 @@
       <c r="B24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="2">
-        <v>404</v>
+      <c r="C24" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>

</xml_diff>

<commit_message>
feat: Update bell_avenue with bingxue, baskin_robbins, mixue
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC5132F-A9A9-40D4-83CA-56580414F5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E8C7E4-CE5F-4F14-ACFD-924EB9E2871D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="2090" windowWidth="19200" windowHeight="10790" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="G" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -843,6 +843,18 @@
   </si>
   <si>
     <t>kk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>br</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bingxue</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mixue</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1057,8 +1069,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1435,8 +1447,8 @@
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="2">
-        <v>404</v>
+      <c r="C22" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1499,8 +1511,8 @@
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="2">
-        <v>404</v>
+      <c r="C26" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2097,8 +2109,8 @@
       <c r="B63" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C63" s="2">
-        <v>404</v>
+      <c r="C63" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>

</xml_diff>

<commit_message>
docs: Change name of jigongbao
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1A_xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A3ED4C-0310-4849-98F0-414E0411C327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462E33CC-FD12-4201-87DC-CDA271544ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="G" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -1105,6 +1105,11 @@
   </si>
   <si>
     <t>billiard</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qianbaiwei Chicken Hot Pot
+千百味鸡煲</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1337,10 +1342,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
+      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -2366,7 +2371,7 @@
     </row>
     <row r="69" spans="1:6" ht="35.25" customHeight="1">
       <c r="A69" s="5" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>8</v>
@@ -2523,9 +2528,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>

</xml_diff>

<commit_message>
docs: Update bell_avenue with heystationery
</commit_message>
<xml_diff>
--- a/src/data/bell_avenue.xlsx
+++ b/src/data/bell_avenue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1A_xmumgithub\xmum-map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462E33CC-FD12-4201-87DC-CDA271544ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ADDF61-014F-41B3-97C4-21D692884E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,27 +102,6 @@
     <t>eathami</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Hey Stationery
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="LXGW WenKai Mono"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>礼品店</t>
-    </r>
-  </si>
-  <si>
     <t>entertainment</t>
   </si>
   <si>
@@ -1110,6 +1089,22 @@
   <si>
     <t>Qianbaiwei Chicken Hot Pot
 千百味鸡煲</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hey Stationery
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>你好同学</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1343,9 +1338,9 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1376,7 +1371,7 @@
     </row>
     <row r="2" spans="1:6" ht="35.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -1393,7 +1388,7 @@
     </row>
     <row r="3" spans="1:6" ht="35.25" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -1436,13 +1431,13 @@
     </row>
     <row r="6" spans="1:6" ht="35.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1453,13 +1448,13 @@
     </row>
     <row r="7" spans="1:6" ht="35.25" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -1478,7 +1473,7 @@
     </row>
     <row r="9" spans="1:6" ht="35.25" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -1503,13 +1498,13 @@
     </row>
     <row r="11" spans="1:6" ht="35.25" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
@@ -1537,13 +1532,13 @@
     </row>
     <row r="13" spans="1:6" ht="35.25" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1571,13 +1566,13 @@
     </row>
     <row r="15" spans="1:6" ht="35.25" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1601,13 +1596,13 @@
     </row>
     <row r="17" spans="1:6" ht="35.25" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1635,13 +1630,13 @@
     </row>
     <row r="19" spans="1:6" ht="35.25" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1652,13 +1647,13 @@
     </row>
     <row r="20" spans="1:6" ht="35.25" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1669,13 +1664,13 @@
     </row>
     <row r="21" spans="1:6" ht="35.25" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1686,13 +1681,13 @@
     </row>
     <row r="22" spans="1:6" ht="35.25" customHeight="1">
       <c r="A22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1716,13 +1711,13 @@
     </row>
     <row r="24" spans="1:6" ht="35.25" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1746,13 +1741,13 @@
     </row>
     <row r="26" spans="1:6" ht="35.25" customHeight="1">
       <c r="A26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1763,13 +1758,13 @@
     </row>
     <row r="27" spans="1:6" ht="35.25" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1780,13 +1775,13 @@
     </row>
     <row r="28" spans="1:6" ht="35.25" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1797,13 +1792,13 @@
     </row>
     <row r="29" spans="1:6" ht="35.25" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1814,13 +1809,13 @@
     </row>
     <row r="30" spans="1:6" ht="35.25" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1831,13 +1826,13 @@
     </row>
     <row r="31" spans="1:6" ht="35.25" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1848,13 +1843,13 @@
     </row>
     <row r="32" spans="1:6" ht="35.25" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1865,13 +1860,13 @@
     </row>
     <row r="33" spans="1:6" ht="35.25" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1895,13 +1890,13 @@
     </row>
     <row r="35" spans="1:6" ht="35.25" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="4" t="b">
@@ -1932,13 +1927,13 @@
     </row>
     <row r="38" spans="1:6" ht="35.25" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -1949,13 +1944,13 @@
     </row>
     <row r="39" spans="1:6" ht="35.25" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -2018,13 +2013,13 @@
     </row>
     <row r="44" spans="1:6" ht="35.25" customHeight="1">
       <c r="A44" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -2074,13 +2069,13 @@
     </row>
     <row r="48" spans="1:6" ht="35.25" customHeight="1">
       <c r="A48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -2091,13 +2086,13 @@
     </row>
     <row r="49" spans="1:6" ht="35.25" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -2108,13 +2103,13 @@
     </row>
     <row r="50" spans="1:6" ht="35.25" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -2138,13 +2133,13 @@
     </row>
     <row r="52" spans="1:6" ht="35.25" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -2155,13 +2150,13 @@
     </row>
     <row r="53" spans="1:6" ht="35.25" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -2185,13 +2180,13 @@
     </row>
     <row r="55" spans="1:6" ht="35.25" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -2202,13 +2197,13 @@
     </row>
     <row r="56" spans="1:6" ht="35.25" customHeight="1">
       <c r="A56" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -2226,13 +2221,13 @@
     </row>
     <row r="58" spans="1:6" ht="35.25" customHeight="1">
       <c r="A58" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D58" s="3">
         <v>2</v>
@@ -2245,13 +2240,13 @@
     </row>
     <row r="59" spans="1:6" ht="35.25" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -2262,13 +2257,13 @@
     </row>
     <row r="60" spans="1:6" ht="35.25" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -2279,13 +2274,13 @@
     </row>
     <row r="61" spans="1:6" ht="35.25" customHeight="1">
       <c r="A61" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -2296,13 +2291,13 @@
     </row>
     <row r="62" spans="1:6" ht="35.25" customHeight="1">
       <c r="A62" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -2313,13 +2308,13 @@
     </row>
     <row r="63" spans="1:6" ht="35.25" customHeight="1">
       <c r="A63" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -2354,13 +2349,13 @@
     </row>
     <row r="68" spans="1:6" ht="35.25" customHeight="1">
       <c r="A68" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -2371,13 +2366,13 @@
     </row>
     <row r="69" spans="1:6" ht="35.25" customHeight="1">
       <c r="A69" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D69" s="3"/>
       <c r="F69" s="4" t="b">
@@ -2394,13 +2389,13 @@
     </row>
     <row r="71" spans="1:6" ht="35.25" customHeight="1">
       <c r="A71" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D71" s="3">
         <v>2</v>
@@ -2413,13 +2408,13 @@
     </row>
     <row r="72" spans="1:6" ht="35.25" customHeight="1">
       <c r="A72" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D72" s="6"/>
       <c r="F72" s="4" t="b">
@@ -2435,13 +2430,13 @@
     </row>
     <row r="74" spans="1:6" ht="35.25" customHeight="1">
       <c r="A74" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -2452,13 +2447,13 @@
     </row>
     <row r="75" spans="1:6" ht="35.25" customHeight="1">
       <c r="A75" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F75" s="4" t="b">
         <f>TRUE()</f>
@@ -2467,7 +2462,7 @@
     </row>
     <row r="76" spans="1:6" ht="35.25" customHeight="1">
       <c r="A76" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>6</v>
@@ -2492,13 +2487,13 @@
     </row>
     <row r="78" spans="1:6" ht="35.25" customHeight="1">
       <c r="A78" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
@@ -2604,13 +2599,13 @@
     </row>
     <row r="6" spans="1:6" ht="35.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -2621,13 +2616,13 @@
     </row>
     <row r="7" spans="1:6" ht="35.25" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -2715,13 +2710,13 @@
     </row>
     <row r="15" spans="1:6" ht="35.25" customHeight="1">
       <c r="A15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2732,13 +2727,13 @@
     </row>
     <row r="16" spans="1:6" ht="35.25" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -2749,13 +2744,13 @@
     </row>
     <row r="17" spans="1:6" ht="35.25" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="1"/>
@@ -2777,13 +2772,13 @@
     </row>
     <row r="19" spans="1:6" ht="35.25" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2794,13 +2789,13 @@
     </row>
     <row r="20" spans="1:6" ht="35.25" customHeight="1">
       <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -2844,13 +2839,13 @@
     </row>
     <row r="24" spans="1:6" ht="35.25" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -2883,13 +2878,13 @@
     </row>
     <row r="27" spans="1:6" ht="35.25" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -2922,13 +2917,13 @@
     </row>
     <row r="30" spans="1:6" ht="35.25" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -3082,13 +3077,13 @@
     </row>
     <row r="44" spans="1:6" ht="35.25" customHeight="1">
       <c r="A44" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D44" s="3">
         <v>2</v>
@@ -3156,13 +3151,13 @@
     </row>
     <row r="50" spans="1:6" ht="35.25" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -3184,13 +3179,13 @@
     </row>
     <row r="52" spans="1:6" ht="35.25" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -3223,13 +3218,13 @@
     </row>
     <row r="55" spans="1:6" ht="35.25" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -3240,13 +3235,13 @@
     </row>
     <row r="56" spans="1:6" ht="35.25" customHeight="1">
       <c r="A56" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -3268,13 +3263,13 @@
     </row>
     <row r="58" spans="1:6" ht="35.25" customHeight="1">
       <c r="A58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -3329,13 +3324,13 @@
     </row>
     <row r="63" spans="1:6" ht="35.25" customHeight="1">
       <c r="A63" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="1"/>
@@ -3346,13 +3341,13 @@
     </row>
     <row r="64" spans="1:6" ht="35.25" customHeight="1">
       <c r="A64" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -3407,13 +3402,13 @@
     </row>
     <row r="69" spans="1:6" ht="35.25" customHeight="1">
       <c r="A69" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -3435,13 +3430,13 @@
     </row>
     <row r="71" spans="1:6" ht="35.25" customHeight="1">
       <c r="A71" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D71" s="3">
         <v>2</v>

</xml_diff>